<commit_message>
Week of 7 November
</commit_message>
<xml_diff>
--- a/data/input/static/base_gis labels.xlsx
+++ b/data/input/static/base_gis labels.xlsx
@@ -510,8 +510,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001F87334A6AC30D4EA6021977FA7E2445" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="13eff9136b4917bb459ad9c1db870f6d">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b370a6fa-a798-42e0-969d-19c284d8683f" xmlns:ns3="62ca1376-8bea-4949-825e-fec085c3924e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="60e7197df19c7150b1ba0c3bfe00adf4" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001F87334A6AC30D4EA6021977FA7E2445" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="504bd14f85abc770ed43885d52246388">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b370a6fa-a798-42e0-969d-19c284d8683f" xmlns:ns3="62ca1376-8bea-4949-825e-fec085c3924e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="823b5556cd3b486fc41cc4ce5ea1e5e3" ns2:_="" ns3:_="">
     <xsd:import namespace="b370a6fa-a798-42e0-969d-19c284d8683f"/>
     <xsd:import namespace="62ca1376-8bea-4949-825e-fec085c3924e"/>
     <xsd:element name="properties">
@@ -529,9 +529,6 @@
                 <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -577,23 +574,6 @@
     <xsd:element name="MediaLengthInSeconds" ma:index="14" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="18" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="19" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="20" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -742,7 +722,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0364A300-2A3D-4EBF-9205-298A7CA0351B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DE1450B-1752-486C-AD50-4AF46B1A1301}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>